<commit_message>
adding colony counts example
</commit_message>
<xml_diff>
--- a/_data_raw/coculture_plate/20250920_v2/diffusion_test_2_samplesheet.xlsx
+++ b/_data_raw/coculture_plate/20250920_v2/diffusion_test_2_samplesheet.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">diffusion_test_media_start</t>
+    <t xml:space="preserve">diffusion_test_M9_start</t>
   </si>
   <si>
     <t xml:space="preserve">B01B02</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">B09</t>
   </si>
   <si>
-    <t xml:space="preserve">double_media</t>
+    <t xml:space="preserve">double_broth</t>
   </si>
   <si>
     <t xml:space="preserve">B09B10</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">E01</t>
   </si>
   <si>
-    <t xml:space="preserve">diffusion_test_salt_start</t>
+    <t xml:space="preserve">diffusion_test_broth_start</t>
   </si>
   <si>
     <t xml:space="preserve">E01E02</t>
@@ -591,13 +591,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.2"/>
@@ -794,6 +794,7 @@
       <c r="H15" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -1606,6 +1607,7 @@
       <c r="H52" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="J52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -1730,7 +1732,7 @@
         <v>23</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>99</v>
@@ -1994,7 +1996,7 @@
         <v>48</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>117</v>
@@ -2258,7 +2260,7 @@
         <v>67</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>135</v>

</xml_diff>